<commit_message>
Update to £888 model to reflect latest changes
</commit_message>
<xml_diff>
--- a/£888.xlsx
+++ b/£888.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7377521D-3009-41FB-B329-E8FA603FA9A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC95EC4-962C-4099-9A14-3E0CB1F9CFA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33525" windowHeight="18900" activeTab="1" xr2:uid="{82812E1B-B9E5-4968-9C43-2C9046B85BEB}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33525" windowHeight="18900" xr2:uid="{82812E1B-B9E5-4968-9C43-2C9046B85BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="192">
   <si>
     <t>Price</t>
   </si>
@@ -594,6 +594,15 @@
   </si>
   <si>
     <t>Market Cap</t>
+  </si>
+  <si>
+    <t>Book Value per Share (GBP)</t>
+  </si>
+  <si>
+    <t>Heavy debt in a high rate environment for WH acquisition</t>
+  </si>
+  <si>
+    <t>Uncertainty over ever-delayed UK Govt. whitepaper on gambling</t>
   </si>
 </sst>
 </file>
@@ -610,7 +619,7 @@
     <numFmt numFmtId="169" formatCode="0.0\x"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +766,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1062,7 +1078,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1287,6 +1303,10 @@
     <xf numFmtId="170" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1341,11 +1361,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1536,7 +1555,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1586,7 +1605,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1926,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0422C3-98AA-4801-8F7F-DD6AC2F99904}">
-  <dimension ref="B2:Q61"/>
+  <dimension ref="B2:S61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21:S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,29 +1968,29 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="142"/>
-      <c r="D5" s="143"/>
-      <c r="I5" s="138" t="s">
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
+      <c r="I5" s="142" t="s">
         <v>129</v>
       </c>
-      <c r="J5" s="139"/>
-      <c r="K5" s="139"/>
-      <c r="L5" s="139"/>
-      <c r="M5" s="139"/>
-      <c r="N5" s="139"/>
-      <c r="O5" s="139"/>
-      <c r="P5" s="139"/>
-      <c r="Q5" s="140"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
+      <c r="N5" s="143"/>
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="69">
-        <v>1.591</v>
+        <v>0.96050000000000002</v>
       </c>
       <c r="D6" s="3"/>
       <c r="I6" s="14" t="s">
@@ -2014,7 +2033,7 @@
       </c>
       <c r="C8" s="69">
         <f>C6*C7</f>
-        <v>647.40223593600001</v>
+        <v>390.84214180800001</v>
       </c>
       <c r="D8" s="3"/>
       <c r="I8" s="13"/>
@@ -2033,7 +2052,7 @@
       </c>
       <c r="C9" s="69">
         <f>299.5*D13</f>
-        <v>248.58499999999998</v>
+        <v>263.56</v>
       </c>
       <c r="D9" s="45" t="s">
         <v>136</v>
@@ -2078,7 +2097,7 @@
       </c>
       <c r="C11" s="69">
         <f>C9-C10</f>
-        <v>248.58499999999998</v>
+        <v>263.56</v>
       </c>
       <c r="D11" s="3"/>
       <c r="I11" s="30" t="s">
@@ -2099,7 +2118,7 @@
       </c>
       <c r="C12" s="70">
         <f>C8-C11</f>
-        <v>398.81723593600003</v>
+        <v>127.28214180800001</v>
       </c>
       <c r="D12" s="4"/>
       <c r="I12" s="30" t="s">
@@ -2115,12 +2134,12 @@
       <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="144" t="s">
+      <c r="B13" s="148" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="145"/>
+      <c r="C13" s="149"/>
       <c r="D13" s="85">
-        <v>0.83</v>
+        <v>0.88</v>
       </c>
       <c r="I13" s="87" t="s">
         <v>145</v>
@@ -2159,11 +2178,11 @@
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="142"/>
-      <c r="D16" s="143"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="147"/>
       <c r="I16" s="30" t="s">
         <v>140</v>
       </c>
@@ -2176,14 +2195,14 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="10"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="152" t="s">
+      <c r="C17" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="153"/>
+      <c r="D17" s="157"/>
       <c r="I17" s="13"/>
       <c r="J17" s="9"/>
       <c r="K17" s="19"/>
@@ -2194,14 +2213,14 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="152" t="s">
+      <c r="C18" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="153"/>
+      <c r="D18" s="157"/>
       <c r="F18" s="25" t="s">
         <v>106</v>
       </c>
@@ -2217,14 +2236,14 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="10"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="152" t="s">
+      <c r="C19" s="156" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="153"/>
+      <c r="D19" s="157"/>
       <c r="F19" t="s">
         <v>107</v>
       </c>
@@ -2240,10 +2259,10 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="10"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="151"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="155"/>
       <c r="F20" t="s">
         <v>108</v>
       </c>
@@ -2257,14 +2276,14 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="10"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="148" t="s">
+      <c r="C21" s="152" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="149"/>
+      <c r="D21" s="153"/>
       <c r="I21" s="14" t="s">
         <v>127</v>
       </c>
@@ -2276,8 +2295,11 @@
       <c r="O21" s="19"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S21" s="163" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I22" s="35" t="s">
         <v>128</v>
       </c>
@@ -2289,8 +2311,11 @@
       <c r="O22" s="19"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="10"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S22" s="163" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I23" s="29" t="s">
         <v>130</v>
       </c>
@@ -2303,12 +2328,12 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="141" t="s">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="145" t="s">
         <v>151</v>
       </c>
-      <c r="C24" s="142"/>
-      <c r="D24" s="143"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="147"/>
       <c r="I24" s="29" t="s">
         <v>131</v>
       </c>
@@ -2321,14 +2346,14 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="152" t="s">
+      <c r="C25" s="156" t="s">
         <v>156</v>
       </c>
-      <c r="D25" s="153"/>
+      <c r="D25" s="157"/>
       <c r="I25" s="13"/>
       <c r="J25" s="9"/>
       <c r="K25" s="19"/>
@@ -2339,14 +2364,14 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="C26" s="152">
+      <c r="C26" s="156">
         <v>1997</v>
       </c>
-      <c r="D26" s="153"/>
+      <c r="D26" s="157"/>
       <c r="I26" s="8" t="s">
         <v>10</v>
       </c>
@@ -2359,7 +2384,7 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="106"/>
       <c r="C27" s="95"/>
       <c r="D27" s="96"/>
@@ -2375,7 +2400,7 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="106"/>
       <c r="C28" s="95"/>
       <c r="D28" s="96"/>
@@ -2391,7 +2416,7 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="106"/>
       <c r="C29" s="95"/>
       <c r="D29" s="96"/>
@@ -2405,14 +2430,14 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="107" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="154" t="s">
+      <c r="C30" s="158" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="155"/>
+      <c r="D30" s="159"/>
       <c r="I30" s="14" t="s">
         <v>13</v>
       </c>
@@ -2425,7 +2450,7 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I31" s="35" t="s">
         <v>63</v>
       </c>
@@ -2438,7 +2463,7 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I32" s="29" t="s">
         <v>64</v>
       </c>
@@ -2452,11 +2477,11 @@
       <c r="Q32" s="10"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="141" t="s">
+      <c r="B33" s="145" t="s">
         <v>186</v>
       </c>
-      <c r="C33" s="142"/>
-      <c r="D33" s="143"/>
+      <c r="C33" s="146"/>
+      <c r="D33" s="147"/>
       <c r="I33" s="12"/>
       <c r="J33" s="9"/>
       <c r="K33" s="19"/>
@@ -2471,11 +2496,11 @@
       <c r="B34" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="C34" s="146">
+      <c r="C34" s="150">
         <f>C6/('Financial Model'!K72*Main!D13)</f>
-        <v>2.4952101532271125</v>
-      </c>
-      <c r="D34" s="147"/>
+        <v>1.4207894993892867</v>
+      </c>
+      <c r="D34" s="151"/>
       <c r="I34" s="14" t="s">
         <v>14</v>
       </c>
@@ -2492,11 +2517,11 @@
       <c r="B35" s="106" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="146">
+      <c r="C35" s="150">
         <f>C6/('Financial Model'!T18*D13)</f>
-        <v>10.332252547239751</v>
-      </c>
-      <c r="D35" s="147"/>
+        <v>5.883254324358421</v>
+      </c>
+      <c r="D35" s="151"/>
       <c r="I35" s="15" t="s">
         <v>15</v>
       </c>
@@ -2867,13 +2892,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E63C3-2D1D-47D3-AA96-4A12957418DF}">
-  <dimension ref="B1:CH78"/>
+  <dimension ref="B1:CH83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H79" sqref="H79"/>
+      <selection pane="bottomRight" activeCell="P81" sqref="P81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5850,7 +5875,7 @@
       </c>
       <c r="AL26" s="66">
         <f>Main!C6</f>
-        <v>1.591</v>
+        <v>0.96050000000000002</v>
       </c>
     </row>
     <row r="27" spans="2:86" x14ac:dyDescent="0.25">
@@ -5916,7 +5941,7 @@
       </c>
       <c r="AL27" s="67">
         <f>AL25/AL26-1</f>
-        <v>4.3642350873440083</v>
+        <v>7.8854742571205811</v>
       </c>
     </row>
     <row r="28" spans="2:86" x14ac:dyDescent="0.25">
@@ -7772,6 +7797,7 @@
       <c r="F70" s="32"/>
       <c r="H70" s="32"/>
       <c r="J70" s="32"/>
+      <c r="L70" s="52"/>
     </row>
     <row r="71" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
@@ -7813,6 +7839,23 @@
         <f t="shared" si="98"/>
         <v>312.59999999999997</v>
       </c>
+      <c r="L71" s="52"/>
+      <c r="Q71">
+        <f t="shared" ref="Q71:T71" si="99">Q43-Q59</f>
+        <v>160.30000000000001</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="99"/>
+        <v>164.7</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="99"/>
+        <v>150.39999999999998</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="99"/>
+        <v>167.89999999999998</v>
+      </c>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
@@ -7823,132 +7866,264 @@
         <v>0.36652385668048432</v>
       </c>
       <c r="D72" s="83">
-        <f t="shared" ref="D72:K72" si="99">D71/D19</f>
+        <f t="shared" ref="D72:K72" si="100">D71/D19</f>
         <v>0.43690239050584234</v>
       </c>
       <c r="E72">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.4160234693761361</v>
       </c>
       <c r="F72" s="83">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.44597614972624322</v>
       </c>
       <c r="G72">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.54604565690197626</v>
       </c>
       <c r="H72" s="83">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.40804373467009325</v>
       </c>
       <c r="I72">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.43577287542557031</v>
       </c>
       <c r="J72" s="83">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.45209379729760402</v>
       </c>
       <c r="K72">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>0.76821884818013808</v>
       </c>
-    </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="H73" s="32"/>
-      <c r="J73" s="32"/>
+      <c r="L72" s="52"/>
+      <c r="Q72">
+        <f t="shared" ref="Q72:T72" si="101">Q71/Q19</f>
+        <v>0.43690239050584234</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="101"/>
+        <v>0.44597614972624322</v>
+      </c>
+      <c r="S72">
+        <f t="shared" si="101"/>
+        <v>0.40804373467009325</v>
+      </c>
+      <c r="T72">
+        <f t="shared" si="101"/>
+        <v>0.45209379729760402</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C73" s="36">
+        <f>C72*(1/C29)</f>
+        <v>0.27750140572417042</v>
+      </c>
+      <c r="D73" s="37">
+        <f t="shared" ref="D73:K73" si="102">D72*(1/D29)</f>
+        <v>0.34418023515506724</v>
+      </c>
+      <c r="E73" s="36">
+        <f t="shared" si="102"/>
+        <v>0.32817186193589654</v>
+      </c>
+      <c r="F73" s="37">
+        <f t="shared" si="102"/>
+        <v>0.34010230284926657</v>
+      </c>
+      <c r="G73" s="36">
+        <f t="shared" si="102"/>
+        <v>0.44354289408007164</v>
+      </c>
+      <c r="H73" s="37">
+        <f t="shared" si="102"/>
+        <v>0.29934981635250041</v>
+      </c>
+      <c r="I73" s="36">
+        <f t="shared" si="102"/>
+        <v>0.31479655813448698</v>
+      </c>
+      <c r="J73" s="37">
+        <f t="shared" si="102"/>
+        <v>0.33493391413365237</v>
+      </c>
+      <c r="K73" s="36">
+        <f t="shared" si="102"/>
+        <v>0.63321698663051273</v>
+      </c>
+      <c r="L73" s="161"/>
+      <c r="U73" s="133"/>
     </row>
     <row r="74" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="D74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="J74" s="32"/>
+      <c r="L74" s="52"/>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>180</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>2.64</v>
       </c>
-      <c r="D74" s="32"/>
-      <c r="E74">
+      <c r="D75" s="32"/>
+      <c r="E75">
         <v>1.63</v>
       </c>
-      <c r="F74" s="32"/>
-      <c r="G74">
+      <c r="F75" s="32"/>
+      <c r="G75">
         <v>1.746</v>
       </c>
-      <c r="H74" s="32"/>
-      <c r="I74">
+      <c r="H75" s="32"/>
+      <c r="I75">
         <v>3.8380000000000001</v>
       </c>
-      <c r="J74" s="32"/>
-      <c r="K74">
+      <c r="J75" s="32"/>
+      <c r="K75">
         <v>1.6759999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="2:21" s="156" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="156" t="s">
+      <c r="L75" s="52"/>
+    </row>
+    <row r="76" spans="2:21" s="138" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="138" t="s">
         <v>188</v>
       </c>
-      <c r="C75" s="159">
-        <f>C74*C19</f>
+      <c r="C76" s="140">
+        <f>C75*C19</f>
         <v>949.32974664000005</v>
       </c>
-      <c r="D75" s="160"/>
-      <c r="E75" s="159">
-        <f>E74*E19</f>
+      <c r="D76" s="141"/>
+      <c r="E76" s="140">
+        <f>E75*E19</f>
         <v>597.50234853999996</v>
       </c>
-      <c r="F75" s="160"/>
-      <c r="G75" s="159">
-        <f>G74*G19</f>
+      <c r="F76" s="141"/>
+      <c r="G76" s="140">
+        <f>G75*G19</f>
         <v>643.34400532199993</v>
       </c>
-      <c r="H75" s="160"/>
-      <c r="I75" s="159">
-        <f>I74*I19</f>
+      <c r="H76" s="141"/>
+      <c r="I76" s="140">
+        <f>I75*I19</f>
         <v>1422.385455714</v>
       </c>
-      <c r="J75" s="160"/>
-      <c r="K75" s="159">
-        <f>K74*K19</f>
+      <c r="J76" s="141"/>
+      <c r="K76" s="140">
+        <f>K75*K19</f>
         <v>681.99003609600004</v>
       </c>
-      <c r="L75" s="157"/>
-      <c r="U75" s="158"/>
-    </row>
-    <row r="76" spans="2:21" s="156" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="156" t="s">
+      <c r="L76" s="52"/>
+      <c r="U76" s="139"/>
+    </row>
+    <row r="77" spans="2:21" s="138" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="C76" s="159">
-        <f>C75-C66</f>
+      <c r="C77" s="140">
+        <f>C76-C66</f>
         <v>804.5297466400001</v>
       </c>
-      <c r="D76" s="160"/>
-      <c r="E76" s="159">
-        <f>E75-E66</f>
+      <c r="D77" s="141"/>
+      <c r="E77" s="140">
+        <f>E76-E66</f>
         <v>544.60234853999998</v>
       </c>
-      <c r="F76" s="160"/>
-      <c r="G76" s="159">
-        <f>G75-G66</f>
+      <c r="F77" s="141"/>
+      <c r="G77" s="140">
+        <f>G76-G66</f>
         <v>501.84400532199993</v>
       </c>
-      <c r="H76" s="160"/>
-      <c r="I76" s="159">
-        <f>I75-I66</f>
+      <c r="H77" s="141"/>
+      <c r="I77" s="140">
+        <f>I76-I66</f>
         <v>1229.485455714</v>
       </c>
-      <c r="J76" s="160"/>
-      <c r="K76" s="159">
-        <f>K75-K66</f>
+      <c r="J77" s="141"/>
+      <c r="K77" s="140">
+        <f>K76-K66</f>
         <v>382.49003609600004</v>
       </c>
-      <c r="L76" s="157"/>
-      <c r="U76" s="158"/>
+      <c r="L77" s="52"/>
+      <c r="U77" s="139"/>
     </row>
     <row r="78" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B78" s="41" t="s">
+      <c r="D78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="H78" s="32"/>
+      <c r="J78" s="32"/>
+      <c r="L78" s="32"/>
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="H79" s="32"/>
+      <c r="J79" s="32"/>
+      <c r="L79" s="32"/>
+    </row>
+    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="160">
+        <f>C75/C73</f>
+        <v>9.5134653214120846</v>
+      </c>
+      <c r="D80" s="162"/>
+      <c r="E80" s="160">
+        <f>E75/E73</f>
+        <v>4.966909686846936</v>
+      </c>
+      <c r="F80" s="162"/>
+      <c r="G80" s="160">
+        <f>G75/G73</f>
+        <v>3.9364851140751207</v>
+      </c>
+      <c r="H80" s="162"/>
+      <c r="I80" s="160">
+        <f>I75/I73</f>
+        <v>12.19200115383833</v>
+      </c>
+      <c r="J80" s="162"/>
+      <c r="K80" s="160">
+        <f>K75/K73</f>
+        <v>2.6468020210865877</v>
+      </c>
+      <c r="L80" s="32"/>
+      <c r="Q80">
+        <f t="shared" ref="Q80:T80" si="103">Q75/Q72</f>
+        <v>0</v>
+      </c>
+      <c r="R80">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="T80">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>187</v>
+      </c>
+      <c r="D81" s="32"/>
+      <c r="F81" s="32"/>
+      <c r="H81" s="32"/>
+      <c r="J81" s="32"/>
+      <c r="L81" s="32"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="41" t="s">
         <v>149</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update £BIDS & £888 with latest developments
</commit_message>
<xml_diff>
--- a/£888.xlsx
+++ b/£888.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC95EC4-962C-4099-9A14-3E0CB1F9CFA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79545C41-C002-40E7-852F-CD1A9AB29085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33525" windowHeight="18900" xr2:uid="{82812E1B-B9E5-4968-9C43-2C9046B85BEB}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="194">
   <si>
     <t>Price</t>
   </si>
@@ -603,6 +603,12 @@
   </si>
   <si>
     <t>Uncertainty over ever-delayed UK Govt. whitepaper on gambling</t>
+  </si>
+  <si>
+    <t>888 Holdings launch 888bet in Kenya, Tanzania, Mozambique &amp; Zambia via 888Africa</t>
+  </si>
+  <si>
+    <t>888Africa hit target of four regulated markets within 6 months of founding business</t>
   </si>
 </sst>
 </file>
@@ -1307,6 +1313,10 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1361,10 +1371,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1945,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0422C3-98AA-4801-8F7F-DD6AC2F99904}">
-  <dimension ref="B2:S61"/>
+  <dimension ref="B2:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21:S22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,22 +1974,22 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="146"/>
-      <c r="D5" s="147"/>
-      <c r="I5" s="142" t="s">
+      <c r="C5" s="150"/>
+      <c r="D5" s="151"/>
+      <c r="I5" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="J5" s="143"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="143"/>
-      <c r="M5" s="143"/>
-      <c r="N5" s="143"/>
-      <c r="O5" s="143"/>
-      <c r="P5" s="143"/>
-      <c r="Q5" s="144"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="148"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
@@ -1994,7 +2000,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="I6" s="14" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="19"/>
@@ -2016,7 +2022,7 @@
         <v>136</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="19"/>
@@ -2058,7 +2064,7 @@
         <v>136</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="19"/>
@@ -2079,8 +2085,8 @@
       <c r="D10" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="I10" s="30" t="s">
-        <v>141</v>
+      <c r="I10" s="29" t="s">
+        <v>150</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="19"/>
@@ -2100,9 +2106,7 @@
         <v>263.56</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="I11" s="30" t="s">
-        <v>142</v>
-      </c>
+      <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
@@ -2121,8 +2125,8 @@
         <v>127.28214180800001</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="I12" s="30" t="s">
-        <v>144</v>
+      <c r="I12" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="19"/>
@@ -2134,15 +2138,15 @@
       <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="152" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="149"/>
+      <c r="C13" s="153"/>
       <c r="D13" s="85">
         <v>0.88</v>
       </c>
-      <c r="I13" s="87" t="s">
-        <v>145</v>
+      <c r="I13" s="30" t="s">
+        <v>141</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="19"/>
@@ -2154,7 +2158,9 @@
       <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I14" s="13"/>
+      <c r="I14" s="30" t="s">
+        <v>142</v>
+      </c>
       <c r="J14" s="9"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
@@ -2165,8 +2171,8 @@
       <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I15" s="14" t="s">
-        <v>139</v>
+      <c r="I15" s="30" t="s">
+        <v>144</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="19"/>
@@ -2178,13 +2184,13 @@
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="145" t="s">
+      <c r="B16" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="146"/>
-      <c r="D16" s="147"/>
-      <c r="I16" s="30" t="s">
-        <v>140</v>
+      <c r="C16" s="150"/>
+      <c r="D16" s="151"/>
+      <c r="I16" s="87" t="s">
+        <v>145</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="19"/>
@@ -2199,10 +2205,10 @@
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="156" t="s">
+      <c r="C17" s="160" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="157"/>
+      <c r="D17" s="161"/>
       <c r="I17" s="13"/>
       <c r="J17" s="9"/>
       <c r="K17" s="19"/>
@@ -2217,15 +2223,15 @@
       <c r="B18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="156" t="s">
+      <c r="C18" s="160" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="157"/>
+      <c r="D18" s="161"/>
       <c r="F18" s="25" t="s">
         <v>106</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="19"/>
@@ -2240,15 +2246,15 @@
       <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="156" t="s">
+      <c r="C19" s="160" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="157"/>
+      <c r="D19" s="161"/>
       <c r="F19" t="s">
         <v>107</v>
       </c>
-      <c r="I19" s="29" t="s">
-        <v>137</v>
+      <c r="I19" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="19"/>
@@ -2261,8 +2267,8 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="154"/>
-      <c r="D20" s="155"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="159"/>
       <c r="F20" t="s">
         <v>108</v>
       </c>
@@ -2280,12 +2286,12 @@
       <c r="B21" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="152" t="s">
+      <c r="C21" s="156" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="153"/>
+      <c r="D21" s="157"/>
       <c r="I21" s="14" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="19"/>
@@ -2295,13 +2301,13 @@
       <c r="O21" s="19"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
-      <c r="S21" s="163" t="s">
+      <c r="S21" s="145" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I22" s="35" t="s">
-        <v>128</v>
+      <c r="I22" s="29" t="s">
+        <v>137</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="19"/>
@@ -2311,14 +2317,12 @@
       <c r="O22" s="19"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="10"/>
-      <c r="S22" s="163" t="s">
+      <c r="S22" s="145" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I23" s="29" t="s">
-        <v>130</v>
-      </c>
+      <c r="I23" s="13"/>
       <c r="J23" s="9"/>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
@@ -2329,13 +2333,13 @@
       <c r="Q23" s="10"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="145" t="s">
+      <c r="B24" s="149" t="s">
         <v>151</v>
       </c>
-      <c r="C24" s="146"/>
-      <c r="D24" s="147"/>
-      <c r="I24" s="29" t="s">
-        <v>131</v>
+      <c r="C24" s="150"/>
+      <c r="D24" s="151"/>
+      <c r="I24" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="19"/>
@@ -2350,11 +2354,13 @@
       <c r="B25" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="156" t="s">
+      <c r="C25" s="160" t="s">
         <v>156</v>
       </c>
-      <c r="D25" s="157"/>
-      <c r="I25" s="13"/>
+      <c r="D25" s="161"/>
+      <c r="I25" s="35" t="s">
+        <v>128</v>
+      </c>
       <c r="J25" s="9"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
@@ -2368,12 +2374,12 @@
       <c r="B26" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="C26" s="156">
+      <c r="C26" s="160">
         <v>1997</v>
       </c>
-      <c r="D26" s="157"/>
-      <c r="I26" s="8" t="s">
-        <v>10</v>
+      <c r="D26" s="161"/>
+      <c r="I26" s="29" t="s">
+        <v>130</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="19"/>
@@ -2388,8 +2394,8 @@
       <c r="B27" s="106"/>
       <c r="C27" s="95"/>
       <c r="D27" s="96"/>
-      <c r="I27" s="11" t="s">
-        <v>11</v>
+      <c r="I27" s="29" t="s">
+        <v>131</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="19"/>
@@ -2404,9 +2410,7 @@
       <c r="B28" s="106"/>
       <c r="C28" s="95"/>
       <c r="D28" s="96"/>
-      <c r="I28" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="I28" s="13"/>
       <c r="J28" s="9"/>
       <c r="K28" s="19"/>
       <c r="L28" s="19"/>
@@ -2420,7 +2424,9 @@
       <c r="B29" s="106"/>
       <c r="C29" s="95"/>
       <c r="D29" s="96"/>
-      <c r="I29" s="13"/>
+      <c r="I29" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="J29" s="9"/>
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
@@ -2434,12 +2440,12 @@
       <c r="B30" s="107" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="158" t="s">
+      <c r="C30" s="162" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="159"/>
-      <c r="I30" s="14" t="s">
-        <v>13</v>
+      <c r="D30" s="163"/>
+      <c r="I30" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="19"/>
@@ -2451,8 +2457,8 @@
       <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I31" s="35" t="s">
-        <v>63</v>
+      <c r="I31" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="19"/>
@@ -2464,9 +2470,7 @@
       <c r="Q31" s="10"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I32" s="29" t="s">
-        <v>64</v>
-      </c>
+      <c r="I32" s="13"/>
       <c r="J32" s="9"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
@@ -2477,12 +2481,14 @@
       <c r="Q32" s="10"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="145" t="s">
+      <c r="B33" s="149" t="s">
         <v>186</v>
       </c>
-      <c r="C33" s="146"/>
-      <c r="D33" s="147"/>
-      <c r="I33" s="12"/>
+      <c r="C33" s="150"/>
+      <c r="D33" s="151"/>
+      <c r="I33" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="J33" s="9"/>
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
@@ -2496,13 +2502,13 @@
       <c r="B34" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="C34" s="150">
+      <c r="C34" s="154">
         <f>C6/('Financial Model'!K72*Main!D13)</f>
         <v>1.4207894993892867</v>
       </c>
-      <c r="D34" s="151"/>
-      <c r="I34" s="14" t="s">
-        <v>14</v>
+      <c r="D34" s="155"/>
+      <c r="I34" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="19"/>
@@ -2517,13 +2523,13 @@
       <c r="B35" s="106" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="150">
+      <c r="C35" s="154">
         <f>C6/('Financial Model'!T18*D13)</f>
         <v>5.883254324358421</v>
       </c>
-      <c r="D35" s="151"/>
-      <c r="I35" s="15" t="s">
-        <v>15</v>
+      <c r="D35" s="155"/>
+      <c r="I35" s="29" t="s">
+        <v>64</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="19"/>
@@ -2535,9 +2541,7 @@
       <c r="Q35" s="10"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I36" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="I36" s="12"/>
       <c r="J36" s="9"/>
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
@@ -2548,8 +2552,8 @@
       <c r="Q36" s="10"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I37" s="12" t="s">
-        <v>17</v>
+      <c r="I37" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="19"/>
@@ -2561,7 +2565,9 @@
       <c r="Q37" s="10"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I38" s="12"/>
+      <c r="I38" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="J38" s="9"/>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
@@ -2572,8 +2578,8 @@
       <c r="Q38" s="10"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I39" s="8" t="s">
-        <v>18</v>
+      <c r="I39" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="19"/>
@@ -2585,8 +2591,8 @@
       <c r="Q39" s="10"/>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I40" s="16" t="s">
-        <v>19</v>
+      <c r="I40" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="J40" s="9"/>
       <c r="K40" s="19"/>
@@ -2598,9 +2604,7 @@
       <c r="Q40" s="10"/>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I41" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="I41" s="12"/>
       <c r="J41" s="9"/>
       <c r="K41" s="19"/>
       <c r="L41" s="19"/>
@@ -2611,8 +2615,8 @@
       <c r="Q41" s="10"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I42" s="15" t="s">
-        <v>21</v>
+      <c r="I42" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="19"/>
@@ -2624,7 +2628,9 @@
       <c r="Q42" s="10"/>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I43" s="13"/>
+      <c r="I43" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="J43" s="9"/>
       <c r="K43" s="19"/>
       <c r="L43" s="19"/>
@@ -2635,8 +2641,8 @@
       <c r="Q43" s="10"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I44" s="17" t="s">
-        <v>22</v>
+      <c r="I44" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="19"/>
@@ -2648,10 +2654,10 @@
       <c r="Q44" s="10"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I45" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J45" s="19"/>
+      <c r="I45" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="9"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
       <c r="M45" s="19"/>
@@ -2661,10 +2667,8 @@
       <c r="Q45" s="10"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I46" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J46" s="19"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="9"/>
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
       <c r="M46" s="19"/>
@@ -2674,10 +2678,10 @@
       <c r="Q46" s="10"/>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I47" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="J47" s="19"/>
+      <c r="I47" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J47" s="9"/>
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
@@ -2688,7 +2692,7 @@
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I48" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J48" s="19"/>
       <c r="K48" s="19"/>
@@ -2700,7 +2704,9 @@
       <c r="Q48" s="10"/>
     </row>
     <row r="49" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I49" s="20"/>
+      <c r="I49" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="J49" s="19"/>
       <c r="K49" s="19"/>
       <c r="L49" s="19"/>
@@ -2711,8 +2717,8 @@
       <c r="Q49" s="10"/>
     </row>
     <row r="50" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I50" s="21" t="s">
-        <v>27</v>
+      <c r="I50" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="J50" s="19"/>
       <c r="K50" s="19"/>
@@ -2724,8 +2730,8 @@
       <c r="Q50" s="10"/>
     </row>
     <row r="51" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I51" s="28" t="s">
-        <v>38</v>
+      <c r="I51" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="J51" s="19"/>
       <c r="K51" s="19"/>
@@ -2737,9 +2743,7 @@
       <c r="Q51" s="10"/>
     </row>
     <row r="52" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I52" s="30" t="s">
-        <v>39</v>
-      </c>
+      <c r="I52" s="20"/>
       <c r="J52" s="19"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
@@ -2750,7 +2754,9 @@
       <c r="Q52" s="10"/>
     </row>
     <row r="53" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I53" s="18"/>
+      <c r="I53" s="21" t="s">
+        <v>27</v>
+      </c>
       <c r="J53" s="19"/>
       <c r="K53" s="19"/>
       <c r="L53" s="19"/>
@@ -2761,8 +2767,8 @@
       <c r="Q53" s="10"/>
     </row>
     <row r="54" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I54" s="21" t="s">
-        <v>28</v>
+      <c r="I54" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="J54" s="19"/>
       <c r="K54" s="19"/>
@@ -2774,8 +2780,8 @@
       <c r="Q54" s="10"/>
     </row>
     <row r="55" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I55" s="28" t="s">
-        <v>37</v>
+      <c r="I55" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
@@ -2788,7 +2794,7 @@
     </row>
     <row r="56" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I56" s="18"/>
-      <c r="J56" s="9"/>
+      <c r="J56" s="19"/>
       <c r="K56" s="19"/>
       <c r="L56" s="19"/>
       <c r="M56" s="19"/>
@@ -2799,9 +2805,9 @@
     </row>
     <row r="57" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I57" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="J57" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="J57" s="19"/>
       <c r="K57" s="19"/>
       <c r="L57" s="19"/>
       <c r="M57" s="19"/>
@@ -2811,10 +2817,10 @@
       <c r="Q57" s="10"/>
     </row>
     <row r="58" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I58" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J58" s="9"/>
+      <c r="I58" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J58" s="19"/>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
       <c r="M58" s="19"/>
@@ -2836,7 +2842,7 @@
     </row>
     <row r="60" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I60" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="19"/>
@@ -2848,17 +2854,54 @@
       <c r="Q60" s="10"/>
     </row>
     <row r="61" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I61" s="22" t="s">
+      <c r="I61" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J61" s="9"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="19"/>
+      <c r="O61" s="19"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="10"/>
+    </row>
+    <row r="62" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I62" s="18"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="19"/>
+      <c r="M62" s="19"/>
+      <c r="N62" s="19"/>
+      <c r="O62" s="19"/>
+      <c r="P62" s="9"/>
+      <c r="Q62" s="10"/>
+    </row>
+    <row r="63" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I63" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J63" s="9"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="10"/>
+    </row>
+    <row r="64" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I64" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J61" s="23"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
-      <c r="M61" s="26"/>
-      <c r="N61" s="26"/>
-      <c r="O61" s="26"/>
-      <c r="P61" s="23"/>
-      <c r="Q61" s="24"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="26"/>
+      <c r="M64" s="26"/>
+      <c r="N64" s="26"/>
+      <c r="O64" s="26"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2880,13 +2923,14 @@
     <mergeCell ref="C26:D26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I9" r:id="rId1" display="UK Government 2022 Legislation" xr:uid="{C1D3F6CD-A120-4B44-833C-73430C0A8313}"/>
-    <hyperlink ref="I6" r:id="rId2" xr:uid="{C680B2B4-B716-DE4A-8BF1-0F084F783051}"/>
+    <hyperlink ref="I12" r:id="rId1" display="UK Government 2022 Legislation" xr:uid="{C1D3F6CD-A120-4B44-833C-73430C0A8313}"/>
+    <hyperlink ref="I9" r:id="rId2" xr:uid="{C680B2B4-B716-DE4A-8BF1-0F084F783051}"/>
     <hyperlink ref="C30:D30" r:id="rId3" location="results-reports-presentations" display="Link" xr:uid="{F059621B-F373-4C60-B0C8-A80A3B8384D6}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{0E5B6056-A23B-4531-AD44-5A14FE0C9AFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -7955,7 +7999,7 @@
         <f t="shared" si="102"/>
         <v>0.63321698663051273</v>
       </c>
-      <c r="L73" s="161"/>
+      <c r="L73" s="143"/>
       <c r="U73" s="133"/>
     </row>
     <row r="74" spans="2:21" x14ac:dyDescent="0.25">
@@ -8070,27 +8114,27 @@
       <c r="B80" t="s">
         <v>185</v>
       </c>
-      <c r="C80" s="160">
+      <c r="C80" s="142">
         <f>C75/C73</f>
         <v>9.5134653214120846</v>
       </c>
-      <c r="D80" s="162"/>
-      <c r="E80" s="160">
+      <c r="D80" s="144"/>
+      <c r="E80" s="142">
         <f>E75/E73</f>
         <v>4.966909686846936</v>
       </c>
-      <c r="F80" s="162"/>
-      <c r="G80" s="160">
+      <c r="F80" s="144"/>
+      <c r="G80" s="142">
         <f>G75/G73</f>
         <v>3.9364851140751207</v>
       </c>
-      <c r="H80" s="162"/>
-      <c r="I80" s="160">
+      <c r="H80" s="144"/>
+      <c r="I80" s="142">
         <f>I75/I73</f>
         <v>12.19200115383833</v>
       </c>
-      <c r="J80" s="162"/>
-      <c r="K80" s="160">
+      <c r="J80" s="144"/>
+      <c r="K80" s="142">
         <f>K75/K73</f>
         <v>2.6468020210865877</v>
       </c>

</xml_diff>

<commit_message>
£888 news event as CEO leaves
</commit_message>
<xml_diff>
--- a/£888.xlsx
+++ b/£888.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307467F2-E4A0-A848-AF1D-35ABDE3C8ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F017239-76CC-41B4-B4F6-1D9A3EDF78E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33520" windowHeight="18900" activeTab="1" xr2:uid="{82812E1B-B9E5-4968-9C43-2C9046B85BEB}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33525" windowHeight="18900" xr2:uid="{82812E1B-B9E5-4968-9C43-2C9046B85BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="201">
   <si>
     <t>Price</t>
   </si>
@@ -634,6 +624,12 @@
   </si>
   <si>
     <t>ROCE</t>
+  </si>
+  <si>
+    <t>888 shares fall 40% as CEO quits following suspension of Middle East VIP service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-exec Chair John Mendelsohn will takeover in the interim </t>
   </si>
 </sst>
 </file>
@@ -641,16 +637,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.0;[Red]\-&quot;£&quot;#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.0\x"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.0;[Red]\-&quot;£&quot;#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,6 +803,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1109,9 +1112,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1132,7 +1135,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1180,7 +1183,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1188,7 +1191,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1199,7 +1202,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1207,11 +1210,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1221,8 +1224,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1234,7 +1237,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1243,9 +1246,9 @@
     <xf numFmtId="14" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1265,9 +1268,9 @@
     <xf numFmtId="14" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1320,32 +1323,32 @@
     <xf numFmtId="14" fontId="15" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1372,10 +1375,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1402,11 +1405,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1984,27 +1997,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0422C3-98AA-4801-8F7F-DD6AC2F99904}">
   <dimension ref="B2:S68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>888</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="151" t="s">
         <v>8</v>
       </c>
@@ -2022,12 +2035,12 @@
       <c r="P5" s="149"/>
       <c r="Q5" s="150"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="69">
-        <v>0.99</v>
+        <v>0.78</v>
       </c>
       <c r="D6" s="3"/>
       <c r="I6" s="13"/>
@@ -2040,7 +2053,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -2050,7 +2063,9 @@
       <c r="D7" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="I7" s="13"/>
+      <c r="I7" s="166" t="s">
+        <v>199</v>
+      </c>
       <c r="J7" s="9"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
@@ -2060,16 +2075,18 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="69">
         <f>C6*C7</f>
-        <v>402.84614304000002</v>
+        <v>317.39393088000003</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="I8" s="13"/>
+      <c r="I8" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="J8" s="9"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
@@ -2079,7 +2096,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
@@ -2099,7 +2116,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
@@ -2121,7 +2138,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
@@ -2142,13 +2159,13 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="70">
         <f>C8-C11</f>
-        <v>2026.84614304</v>
+        <v>1941.39393088</v>
       </c>
       <c r="D12" s="4"/>
       <c r="I12" s="13"/>
@@ -2161,7 +2178,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="154" t="s">
         <v>132</v>
       </c>
@@ -2181,7 +2198,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I14" s="29" t="s">
         <v>150</v>
       </c>
@@ -2194,7 +2211,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="10"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I15" s="13"/>
       <c r="J15" s="9"/>
       <c r="K15" s="19"/>
@@ -2205,7 +2222,7 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="10"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="151" t="s">
         <v>9</v>
       </c>
@@ -2223,14 +2240,14 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="10"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="162" t="s">
+      <c r="C17" s="168" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="163"/>
+      <c r="D17" s="169"/>
       <c r="I17" s="30" t="s">
         <v>141</v>
       </c>
@@ -2243,7 +2260,7 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>34</v>
       </c>
@@ -2266,7 +2283,7 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="10"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
@@ -2289,7 +2306,7 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="10"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="160"/>
       <c r="D20" s="161"/>
@@ -2308,7 +2325,7 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="10"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
         <v>36</v>
       </c>
@@ -2329,7 +2346,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I22" s="14" t="s">
         <v>139</v>
       </c>
@@ -2345,7 +2362,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I23" s="30" t="s">
         <v>140</v>
       </c>
@@ -2358,7 +2375,7 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="151" t="s">
         <v>151</v>
       </c>
@@ -2374,7 +2391,7 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="106" t="s">
         <v>154</v>
       </c>
@@ -2394,7 +2411,7 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="106" t="s">
         <v>155</v>
       </c>
@@ -2414,7 +2431,7 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="106"/>
       <c r="C27" s="95"/>
       <c r="D27" s="96"/>
@@ -2428,7 +2445,7 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="106"/>
       <c r="C28" s="95"/>
       <c r="D28" s="96"/>
@@ -2444,7 +2461,7 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="106"/>
       <c r="C29" s="95"/>
       <c r="D29" s="96"/>
@@ -2460,7 +2477,7 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="107" t="s">
         <v>152</v>
       </c>
@@ -2480,7 +2497,7 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I31" s="29" t="s">
         <v>131</v>
       </c>
@@ -2493,7 +2510,7 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I32" s="13"/>
       <c r="J32" s="9"/>
       <c r="K32" s="19"/>
@@ -2504,7 +2521,7 @@
       <c r="P32" s="9"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="151" t="s">
         <v>186</v>
       </c>
@@ -2522,13 +2539,13 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="106" t="s">
         <v>185</v>
       </c>
       <c r="C34" s="156">
         <f>C6/('Financial Model'!K72*Main!D13)</f>
-        <v>1.4644264491362766</v>
+        <v>1.1537905356831271</v>
       </c>
       <c r="D34" s="157"/>
       <c r="I34" s="11" t="s">
@@ -2543,13 +2560,13 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="106" t="s">
         <v>187</v>
       </c>
       <c r="C35" s="156">
         <f>C6/('Financial Model'!T18*D13)</f>
-        <v>6.0639477158925938</v>
+        <v>4.7776557761578013</v>
       </c>
       <c r="D35" s="157"/>
       <c r="I35" s="12" t="s">
@@ -2564,7 +2581,7 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="106"/>
       <c r="C36" s="146"/>
       <c r="D36" s="147"/>
@@ -2578,7 +2595,7 @@
       <c r="P36" s="9"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="106" t="s">
         <v>185</v>
       </c>
@@ -2596,7 +2613,7 @@
       <c r="P37" s="9"/>
       <c r="Q37" s="10"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="106" t="s">
         <v>195</v>
       </c>
@@ -2614,7 +2631,7 @@
       <c r="P38" s="9"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="106" t="s">
         <v>196</v>
       </c>
@@ -2632,7 +2649,7 @@
       <c r="P39" s="9"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="106" t="s">
         <v>187</v>
       </c>
@@ -2648,7 +2665,7 @@
       <c r="P40" s="9"/>
       <c r="Q40" s="10"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="106" t="s">
         <v>197</v>
       </c>
@@ -2666,7 +2683,7 @@
       <c r="P41" s="9"/>
       <c r="Q41" s="10"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="106" t="s">
         <v>198</v>
       </c>
@@ -2684,7 +2701,7 @@
       <c r="P42" s="9"/>
       <c r="Q42" s="10"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I43" s="12" t="s">
         <v>16</v>
       </c>
@@ -2697,7 +2714,7 @@
       <c r="P43" s="9"/>
       <c r="Q43" s="10"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I44" s="12" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +2727,7 @@
       <c r="P44" s="9"/>
       <c r="Q44" s="10"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I45" s="12"/>
       <c r="J45" s="9"/>
       <c r="K45" s="19"/>
@@ -2721,7 +2738,7 @@
       <c r="P45" s="9"/>
       <c r="Q45" s="10"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I46" s="8" t="s">
         <v>18</v>
       </c>
@@ -2734,7 +2751,7 @@
       <c r="P46" s="9"/>
       <c r="Q46" s="10"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I47" s="16" t="s">
         <v>19</v>
       </c>
@@ -2747,7 +2764,7 @@
       <c r="P47" s="9"/>
       <c r="Q47" s="10"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I48" s="12" t="s">
         <v>20</v>
       </c>
@@ -2760,7 +2777,7 @@
       <c r="P48" s="9"/>
       <c r="Q48" s="10"/>
     </row>
-    <row r="49" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I49" s="15" t="s">
         <v>21</v>
       </c>
@@ -2773,7 +2790,7 @@
       <c r="P49" s="9"/>
       <c r="Q49" s="10"/>
     </row>
-    <row r="50" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I50" s="13"/>
       <c r="J50" s="9"/>
       <c r="K50" s="19"/>
@@ -2784,7 +2801,7 @@
       <c r="P50" s="9"/>
       <c r="Q50" s="10"/>
     </row>
-    <row r="51" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I51" s="17" t="s">
         <v>22</v>
       </c>
@@ -2797,7 +2814,7 @@
       <c r="P51" s="9"/>
       <c r="Q51" s="10"/>
     </row>
-    <row r="52" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I52" s="18" t="s">
         <v>23</v>
       </c>
@@ -2810,7 +2827,7 @@
       <c r="P52" s="9"/>
       <c r="Q52" s="10"/>
     </row>
-    <row r="53" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I53" s="18" t="s">
         <v>24</v>
       </c>
@@ -2823,7 +2840,7 @@
       <c r="P53" s="9"/>
       <c r="Q53" s="10"/>
     </row>
-    <row r="54" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I54" s="20" t="s">
         <v>25</v>
       </c>
@@ -2836,7 +2853,7 @@
       <c r="P54" s="9"/>
       <c r="Q54" s="10"/>
     </row>
-    <row r="55" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I55" s="18" t="s">
         <v>26</v>
       </c>
@@ -2849,7 +2866,7 @@
       <c r="P55" s="9"/>
       <c r="Q55" s="10"/>
     </row>
-    <row r="56" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I56" s="20"/>
       <c r="J56" s="19"/>
       <c r="K56" s="19"/>
@@ -2860,7 +2877,7 @@
       <c r="P56" s="9"/>
       <c r="Q56" s="10"/>
     </row>
-    <row r="57" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I57" s="21" t="s">
         <v>27</v>
       </c>
@@ -2873,7 +2890,7 @@
       <c r="P57" s="9"/>
       <c r="Q57" s="10"/>
     </row>
-    <row r="58" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I58" s="28" t="s">
         <v>38</v>
       </c>
@@ -2886,7 +2903,7 @@
       <c r="P58" s="9"/>
       <c r="Q58" s="10"/>
     </row>
-    <row r="59" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I59" s="30" t="s">
         <v>39</v>
       </c>
@@ -2899,7 +2916,7 @@
       <c r="P59" s="9"/>
       <c r="Q59" s="10"/>
     </row>
-    <row r="60" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I60" s="18"/>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
@@ -2910,7 +2927,7 @@
       <c r="P60" s="9"/>
       <c r="Q60" s="10"/>
     </row>
-    <row r="61" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I61" s="21" t="s">
         <v>28</v>
       </c>
@@ -2923,7 +2940,7 @@
       <c r="P61" s="9"/>
       <c r="Q61" s="10"/>
     </row>
-    <row r="62" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I62" s="28" t="s">
         <v>37</v>
       </c>
@@ -2936,7 +2953,7 @@
       <c r="P62" s="9"/>
       <c r="Q62" s="10"/>
     </row>
-    <row r="63" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I63" s="18"/>
       <c r="J63" s="9"/>
       <c r="K63" s="19"/>
@@ -2947,7 +2964,7 @@
       <c r="P63" s="9"/>
       <c r="Q63" s="10"/>
     </row>
-    <row r="64" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I64" s="21" t="s">
         <v>29</v>
       </c>
@@ -2960,7 +2977,7 @@
       <c r="P64" s="9"/>
       <c r="Q64" s="10"/>
     </row>
-    <row r="65" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I65" s="18" t="s">
         <v>30</v>
       </c>
@@ -2973,7 +2990,7 @@
       <c r="P65" s="9"/>
       <c r="Q65" s="10"/>
     </row>
-    <row r="66" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I66" s="18"/>
       <c r="J66" s="9"/>
       <c r="K66" s="19"/>
@@ -2984,7 +3001,7 @@
       <c r="P66" s="9"/>
       <c r="Q66" s="10"/>
     </row>
-    <row r="67" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I67" s="21" t="s">
         <v>31</v>
       </c>
@@ -2997,7 +3014,7 @@
       <c r="P67" s="9"/>
       <c r="Q67" s="10"/>
     </row>
-    <row r="68" spans="9:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I68" s="22" t="s">
         <v>32</v>
       </c>
@@ -3034,10 +3051,11 @@
     <hyperlink ref="I13" r:id="rId2" xr:uid="{C680B2B4-B716-DE4A-8BF1-0F084F783051}"/>
     <hyperlink ref="C30:D30" r:id="rId3" location="results-reports-presentations" display="Link" xr:uid="{F059621B-F373-4C60-B0C8-A80A3B8384D6}"/>
     <hyperlink ref="I10" r:id="rId4" xr:uid="{0E5B6056-A23B-4531-AD44-5A14FE0C9AFF}"/>
+    <hyperlink ref="I7" r:id="rId5" display="888 shares fall 30% as CEO quits following suspension of Middle East VIP service" xr:uid="{C60967F6-59D8-4026-8FC5-7B67BB9C7214}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3045,27 +3063,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E63C3-2D1D-47D3-AA96-4A12957418DF}">
   <dimension ref="B1:CH83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="92"/>
-    <col min="17" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" style="102"/>
-    <col min="37" max="37" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="92"/>
+    <col min="17" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" style="102"/>
+    <col min="37" max="37" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B1" s="38" t="s">
         <v>75</v>
       </c>
@@ -3157,7 +3175,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C2" s="50">
         <v>43281</v>
       </c>
@@ -3249,7 +3267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>58</v>
       </c>
@@ -3361,7 +3379,7 @@
         <v>2355.0858710106172</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3472,7 +3490,7 @@
         <v>442.13427228441333</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3587,7 +3605,7 @@
         <v>380.61993874919068</v>
       </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
         <v>73</v>
       </c>
@@ -3707,7 +3725,7 @@
         <v>822.75421103360395</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>74</v>
       </c>
@@ -3827,7 +3845,7 @@
         <v>1532.3316599770133</v>
       </c>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8" s="36" t="s">
         <v>76</v>
       </c>
@@ -3938,7 +3956,7 @@
         <v>594.38587131986117</v>
       </c>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9" s="36" t="s">
         <v>77</v>
       </c>
@@ -4049,7 +4067,7 @@
         <v>427.02697835116948</v>
       </c>
     </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="36" t="s">
         <v>78</v>
       </c>
@@ -4160,7 +4178,7 @@
         <v>49.952205219311665</v>
       </c>
     </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>79</v>
       </c>
@@ -4280,7 +4298,7 @@
         <v>460.96660508667094</v>
       </c>
     </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B12" s="36" t="s">
         <v>80</v>
       </c>
@@ -4377,7 +4395,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B13" s="36" t="s">
         <v>81</v>
       </c>
@@ -4474,7 +4492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B14" s="36" t="s">
         <v>82</v>
       </c>
@@ -4572,7 +4590,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B15" s="36" t="s">
         <v>83</v>
       </c>
@@ -4692,7 +4710,7 @@
         <v>454.96660508667094</v>
       </c>
     </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B16" s="36" t="s">
         <v>84</v>
       </c>
@@ -4803,7 +4821,7 @@
         <v>28.261030452127407</v>
       </c>
     </row>
-    <row r="17" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>85</v>
       </c>
@@ -5134,7 +5152,7 @@
         <v>87.550473357948007</v>
       </c>
     </row>
-    <row r="18" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B18" s="36" t="s">
         <v>86</v>
       </c>
@@ -5254,7 +5272,7 @@
         <v>1.1542526881293376</v>
       </c>
     </row>
-    <row r="19" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
@@ -5365,7 +5383,7 @@
         <v>369.68124832881472</v>
       </c>
     </row>
-    <row r="20" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:86" x14ac:dyDescent="0.25">
       <c r="D20" s="37"/>
       <c r="F20" s="37"/>
       <c r="H20" s="32"/>
@@ -5381,7 +5399,7 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="21" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -5507,7 +5525,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>69</v>
       </c>
@@ -5634,7 +5652,7 @@
         <v>3217.2177896328553</v>
       </c>
     </row>
-    <row r="23" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>68</v>
       </c>
@@ -5760,7 +5778,7 @@
         <v>255.6</v>
       </c>
     </row>
-    <row r="24" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>67</v>
       </c>
@@ -5887,7 +5905,7 @@
         <v>3472.8177896328552</v>
       </c>
     </row>
-    <row r="25" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:86" x14ac:dyDescent="0.25">
       <c r="D25" s="37"/>
       <c r="F25" s="37"/>
       <c r="H25" s="37"/>
@@ -5902,7 +5920,7 @@
         <v>8.5344980239643178</v>
       </c>
     </row>
-    <row r="26" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
         <v>65</v>
       </c>
@@ -6026,10 +6044,10 @@
       </c>
       <c r="AL26" s="66">
         <f>Main!C6</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="27" spans="2:86" x14ac:dyDescent="0.2">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B27" s="36" t="s">
         <v>66</v>
       </c>
@@ -6092,10 +6110,10 @@
       </c>
       <c r="AL27" s="67">
         <f>AL25/AL26-1</f>
-        <v>7.6207050747114327</v>
-      </c>
-    </row>
-    <row r="28" spans="2:86" x14ac:dyDescent="0.2">
+        <v>9.9416641332875866</v>
+      </c>
+    </row>
+    <row r="28" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B28" s="36"/>
       <c r="C28" s="54"/>
       <c r="D28" s="52"/>
@@ -6107,7 +6125,7 @@
       <c r="J28" s="52"/>
       <c r="L28" s="32"/>
     </row>
-    <row r="29" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B29" s="36" t="s">
         <v>133</v>
       </c>
@@ -6152,7 +6170,7 @@
         <v>1.3498000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B30" s="36" t="s">
         <v>157</v>
       </c>
@@ -6208,14 +6226,14 @@
         <v>-9.7571711539871098E-3</v>
       </c>
     </row>
-    <row r="31" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:86" x14ac:dyDescent="0.25">
       <c r="D31" s="32"/>
       <c r="F31" s="32"/>
       <c r="H31" s="59"/>
       <c r="J31" s="32"/>
       <c r="L31" s="32"/>
     </row>
-    <row r="32" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B32" s="41" t="s">
         <v>87</v>
       </c>
@@ -6225,7 +6243,7 @@
       <c r="J32" s="32"/>
       <c r="L32" s="32"/>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="36" t="s">
         <v>89</v>
       </c>
@@ -6274,7 +6292,7 @@
         <v>167.2</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="36" t="s">
         <v>90</v>
       </c>
@@ -6323,7 +6341,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="36" t="s">
         <v>91</v>
       </c>
@@ -6372,7 +6390,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="36" t="s">
         <v>111</v>
       </c>
@@ -6421,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="36" t="s">
         <v>92</v>
       </c>
@@ -6470,7 +6488,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="36" t="s">
         <v>93</v>
       </c>
@@ -6519,7 +6537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>88</v>
       </c>
@@ -6577,7 +6595,7 @@
         <v>215.9</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="25" t="s">
         <v>3</v>
       </c>
@@ -6630,7 +6648,7 @@
         <v>255.6</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>94</v>
       </c>
@@ -6679,7 +6697,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>181</v>
       </c>
@@ -6724,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -6782,14 +6800,14 @@
         <v>540</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D44" s="32"/>
       <c r="F44" s="32"/>
       <c r="H44" s="59"/>
       <c r="J44" s="32"/>
       <c r="L44" s="32"/>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>96</v>
       </c>
@@ -6838,7 +6856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>93</v>
       </c>
@@ -6887,7 +6905,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>97</v>
       </c>
@@ -6936,7 +6954,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="48" spans="2:21" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
         <v>110</v>
       </c>
@@ -6986,7 +7004,7 @@
       </c>
       <c r="U48" s="105"/>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>98</v>
       </c>
@@ -7044,14 +7062,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D50" s="32"/>
       <c r="F50" s="32"/>
       <c r="H50" s="59"/>
       <c r="J50" s="32"/>
       <c r="L50" s="32"/>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>99</v>
       </c>
@@ -7100,7 +7118,7 @@
         <v>196.1</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>100</v>
       </c>
@@ -7149,7 +7167,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>101</v>
       </c>
@@ -7199,7 +7217,7 @@
         <v>30.7</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>97</v>
       </c>
@@ -7248,7 +7266,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="55" spans="2:21" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="25" t="s">
         <v>110</v>
       </c>
@@ -7298,7 +7316,7 @@
       </c>
       <c r="U55" s="105"/>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>96</v>
       </c>
@@ -7347,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B57" s="25" t="s">
         <v>102</v>
       </c>
@@ -7400,7 +7418,7 @@
         <v>81.099999999999994</v>
       </c>
     </row>
-    <row r="58" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="36" t="s">
         <v>182</v>
       </c>
@@ -7446,7 +7464,7 @@
       </c>
       <c r="U58" s="133"/>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>105</v>
       </c>
@@ -7504,14 +7522,14 @@
         <v>372.1</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D60" s="32"/>
       <c r="F60" s="32"/>
       <c r="H60" s="59"/>
       <c r="J60" s="32"/>
       <c r="L60" s="32"/>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>103</v>
       </c>
@@ -7560,7 +7578,7 @@
         <v>167.9</v>
       </c>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>104</v>
       </c>
@@ -7618,14 +7636,14 @@
         <v>540</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D63" s="32"/>
       <c r="F63" s="32"/>
       <c r="H63" s="32"/>
       <c r="J63" s="32"/>
       <c r="L63" s="32"/>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B64" s="77" t="s">
         <v>3</v>
       </c>
@@ -7687,7 +7705,7 @@
         <v>255.6</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B65" s="80" t="s">
         <v>4</v>
       </c>
@@ -7749,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:21" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="108" t="s">
         <v>5</v>
       </c>
@@ -7812,14 +7830,14 @@
       </c>
       <c r="U66" s="105"/>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D67" s="32"/>
       <c r="F67" s="32"/>
       <c r="H67" s="32"/>
       <c r="J67" s="32"/>
       <c r="L67" s="32"/>
     </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>135</v>
       </c>
@@ -7881,7 +7899,7 @@
         <v>3.1516646115906291</v>
       </c>
     </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>134</v>
       </c>
@@ -7943,14 +7961,14 @@
         <v>3.1516646115906291</v>
       </c>
     </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D70" s="32"/>
       <c r="F70" s="32"/>
       <c r="H70" s="32"/>
       <c r="J70" s="32"/>
       <c r="L70" s="52"/>
     </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>183</v>
       </c>
@@ -8008,7 +8026,7 @@
         <v>167.89999999999998</v>
       </c>
     </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>184</v>
       </c>
@@ -8066,7 +8084,7 @@
         <v>0.45209379729760402</v>
       </c>
     </row>
-    <row r="73" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="36" t="s">
         <v>189</v>
       </c>
@@ -8109,14 +8127,14 @@
       <c r="L73" s="143"/>
       <c r="U73" s="133"/>
     </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D74" s="32"/>
       <c r="F74" s="32"/>
       <c r="H74" s="32"/>
       <c r="J74" s="32"/>
       <c r="L74" s="52"/>
     </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>180</v>
       </c>
@@ -8141,7 +8159,7 @@
       </c>
       <c r="L75" s="52"/>
     </row>
-    <row r="76" spans="2:21" s="138" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:21" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="138" t="s">
         <v>188</v>
       </c>
@@ -8172,7 +8190,7 @@
       <c r="L76" s="52"/>
       <c r="U76" s="139"/>
     </row>
-    <row r="77" spans="2:21" s="138" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:21" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="138" t="s">
         <v>6</v>
       </c>
@@ -8203,21 +8221,21 @@
       <c r="L77" s="52"/>
       <c r="U77" s="139"/>
     </row>
-    <row r="78" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D78" s="32"/>
       <c r="F78" s="32"/>
       <c r="H78" s="32"/>
       <c r="J78" s="32"/>
       <c r="L78" s="32"/>
     </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D79" s="32"/>
       <c r="F79" s="32"/>
       <c r="H79" s="32"/>
       <c r="J79" s="32"/>
       <c r="L79" s="32"/>
     </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>185</v>
       </c>
@@ -8263,7 +8281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>187</v>
       </c>
@@ -8273,7 +8291,7 @@
       <c r="J81" s="32"/>
       <c r="L81" s="32"/>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="41" t="s">
         <v>149</v>
       </c>
@@ -8296,18 +8314,18 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="112" t="s">
         <v>158</v>
       </c>
@@ -8330,7 +8348,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="113">
         <v>44785</v>
       </c>
@@ -8350,7 +8368,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="117">
         <v>44768</v>
       </c>
@@ -8370,7 +8388,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="113">
         <v>44762</v>
       </c>
@@ -8390,7 +8408,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="117">
         <v>44747</v>
       </c>
@@ -8410,7 +8428,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="113">
         <v>44697</v>
       </c>
@@ -8430,7 +8448,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="117">
         <v>44665</v>
       </c>
@@ -8450,7 +8468,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="113">
         <v>44658</v>
       </c>
@@ -8470,7 +8488,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="117">
         <v>44650</v>
       </c>
@@ -8490,7 +8508,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="113">
         <v>44642</v>
       </c>
@@ -8510,7 +8528,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="117">
         <v>44629</v>
       </c>
@@ -8530,7 +8548,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="113">
         <v>44629</v>
       </c>
@@ -8550,7 +8568,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="117">
         <v>44578</v>
       </c>
@@ -8570,7 +8588,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="113">
         <v>44531</v>
       </c>
@@ -8590,7 +8608,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="117">
         <v>44530</v>
       </c>
@@ -8610,7 +8628,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="113">
         <v>44488</v>
       </c>
@@ -8630,7 +8648,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="117">
         <v>44488</v>
       </c>
@@ -8650,7 +8668,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="113">
         <v>44488</v>
       </c>
@@ -8670,7 +8688,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="117">
         <v>44469</v>
       </c>
@@ -8690,7 +8708,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="113">
         <v>44449</v>
       </c>
@@ -8710,7 +8728,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="117">
         <v>44439</v>
       </c>
@@ -8730,7 +8748,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="113">
         <v>44383</v>
       </c>
@@ -8750,7 +8768,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="117">
         <v>44371</v>
       </c>
@@ -8770,7 +8788,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="113">
         <v>44371</v>
       </c>
@@ -8790,7 +8808,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="117">
         <v>44314</v>
       </c>
@@ -8810,7 +8828,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="113">
         <v>44314</v>
       </c>
@@ -8830,7 +8848,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="117">
         <v>44285</v>
       </c>
@@ -8850,7 +8868,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="113">
         <v>44273</v>
       </c>
@@ -8870,7 +8888,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="117">
         <v>44273</v>
       </c>
@@ -8890,7 +8908,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="113">
         <v>44252</v>
       </c>
@@ -8910,7 +8928,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="117">
         <v>44011</v>
       </c>
@@ -8930,7 +8948,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="113">
         <v>44011</v>
       </c>
@@ -8950,7 +8968,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="117">
         <v>43837</v>
       </c>
@@ -8970,7 +8988,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="113">
         <v>43718</v>
       </c>
@@ -8990,7 +9008,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="117">
         <v>43642</v>
       </c>
@@ -9010,7 +9028,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="113">
         <v>43622</v>
       </c>
@@ -9030,7 +9048,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="117">
         <v>43621</v>
       </c>
@@ -9050,7 +9068,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="113">
         <v>43613</v>
       </c>
@@ -9070,7 +9088,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="117">
         <v>43536</v>
       </c>
@@ -9090,7 +9108,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="113">
         <v>43528</v>
       </c>
@@ -9110,7 +9128,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="117">
         <v>43453</v>
       </c>
@@ -9130,7 +9148,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="113">
         <v>43453</v>
       </c>
@@ -9150,7 +9168,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="117">
         <v>43423</v>
       </c>
@@ -9170,7 +9188,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="113">
         <v>43402</v>
       </c>
@@ -9190,7 +9208,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="117">
         <v>43370</v>
       </c>
@@ -9210,7 +9228,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="113">
         <v>43370</v>
       </c>
@@ -9230,7 +9248,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="117">
         <v>43353</v>
       </c>
@@ -9250,7 +9268,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="113">
         <v>43321</v>
       </c>
@@ -9270,7 +9288,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="117">
         <v>43238</v>
       </c>
@@ -9290,7 +9308,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="113">
         <v>43179</v>
       </c>
@@ -9310,7 +9328,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="117">
         <v>42983</v>
       </c>

</xml_diff>